<commit_message>
demand measurements also added
</commit_message>
<xml_diff>
--- a/src/master_data/scada_files_info_master.xlsx
+++ b/src/master_data/scada_files_info_master.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20352"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B51335-BC54-4D7A-979D-962C4E5F3394}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F47D272F-2741-4916-B9A2-A5F252D5E771}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2623" uniqueCount="1675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2750" uniqueCount="1739">
   <si>
     <t>Id</t>
   </si>
@@ -5044,6 +5044,198 @@
   </si>
   <si>
     <t>S:\volttemp</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>S:\DEMAND</t>
+  </si>
+  <si>
+    <t>Demand_</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046980</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MSEB_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>RCTMH_WR.SYSTEM.MUM_DEMAND.MEAS.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046957</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.GEB_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046978</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MPSEB_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046945</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.CSEB_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046962</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.GOA_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046948</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.DD_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046953</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.DNH_DEMAND.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046960</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.GEB_TOT_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046984</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MSEB_TOT_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046979</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MPSEB_TOT_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046947</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.CSEB_TOT_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046958</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.GEB_HYDRO_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046959</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.GEB_TH_GS_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046981</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MSEB_HYD_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046982</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MSEB_TH_GS_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0047287</t>
+  </si>
+  <si>
+    <t>SUBSTN.MPRTC_MP.STTN.TOTHYD_MW.MEAS.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046992</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.THRML_MW.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046946</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.CSEB_HYDRO_MW.MEAS.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046391</t>
+  </si>
+  <si>
+    <t>SUBSTN.SYSCA_CG.SYSTEM.ALL_GEN_CG_MW.MEAS.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046999</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.WR_NUCLEAR_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0047002</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.WR_TOT_HYD_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0047003</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.WR_TOT_TH_GS.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046961</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.GEB_TRML_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0046983</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.MSEB_THRM_GEN.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0047004</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.WR_TOT_TH_ONLY.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA1.A0049839</t>
+  </si>
+  <si>
+    <t>SUBSTN.ATHN4_IP.STTN.USER_CALC.MEAS.UC1</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA3.A0109531</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.TOT_WIND_MH.ADDT.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA3.A0108220</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.TOT_SOLAR_MH.ADD.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA3.A0106536</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.ABT.ALL_INDIA_DMD.MEAS.MW</t>
+  </si>
+  <si>
+    <t>WRLDCMP.SCADA3.A0111629</t>
+  </si>
+  <si>
+    <t>SUBSTN.IMEXP_WR.SYSTEM.BARC_TOTAL.ADDT.MW</t>
   </si>
 </sst>
 </file>
@@ -5459,10 +5651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5671,6 +5863,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1676</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1677</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="\\10.2.100.51\scada\Reports\ICT" xr:uid="{8F96B5CA-F2D3-46BB-ADEF-22399229D1CA}"/>
@@ -5678,6 +5902,7 @@
     <hyperlink ref="B5" r:id="rId3" display="\\10.2.100.51\scada\Reports\ONEMINREPORT" xr:uid="{2719DF97-17AA-4851-AE5F-8796CDD2EC83}"/>
     <hyperlink ref="B6" r:id="rId4" display="\\10.2.100.51\scada\Reports\State_gen" xr:uid="{5A859482-7B67-4E67-869F-1BB440ABEB5C}"/>
     <hyperlink ref="B2" r:id="rId5" display="\\10.2.100.51\scada\Reports\volttemp" xr:uid="{182E7FE1-B692-42CF-8B87-8CB0E1931C4E}"/>
+    <hyperlink ref="B7" r:id="rId6" display="\\10.2.100.51\scada\Reports\State_gen" xr:uid="{F966EFD5-41ED-40CE-8090-217F9FA2BABC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5685,10 +5910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D859"/>
+  <dimension ref="A1:D899"/>
   <sheetViews>
-    <sheetView topLeftCell="A829" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D838" sqref="D838"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17724,6 +17949,566 @@
         <v>1663</v>
       </c>
     </row>
+    <row r="860" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A860" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B860">
+        <v>2</v>
+      </c>
+      <c r="C860" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D860" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="861" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A861" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B861">
+        <v>3</v>
+      </c>
+      <c r="C861" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D861" t="s">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="862" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A862" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B862">
+        <v>4</v>
+      </c>
+      <c r="C862" t="s">
+        <v>1678</v>
+      </c>
+      <c r="D862" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="863" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A863" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B863">
+        <v>5</v>
+      </c>
+      <c r="C863" t="s">
+        <v>1512</v>
+      </c>
+      <c r="D863" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="864" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A864" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B864">
+        <v>6</v>
+      </c>
+      <c r="C864" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D864" t="s">
+        <v>1682</v>
+      </c>
+    </row>
+    <row r="865" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A865" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B865">
+        <v>7</v>
+      </c>
+      <c r="C865" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D865" t="s">
+        <v>1684</v>
+      </c>
+    </row>
+    <row r="866" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A866" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B866">
+        <v>8</v>
+      </c>
+      <c r="C866" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D866" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="867" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A867" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B867">
+        <v>9</v>
+      </c>
+      <c r="C867" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D867" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="868" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A868" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B868">
+        <v>10</v>
+      </c>
+      <c r="C868" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D868" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="869" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A869" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B869">
+        <v>11</v>
+      </c>
+      <c r="C869" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D869" t="s">
+        <v>1692</v>
+      </c>
+    </row>
+    <row r="870" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A870" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B870">
+        <v>12</v>
+      </c>
+      <c r="C870" t="s">
+        <v>1693</v>
+      </c>
+      <c r="D870" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="871" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A871" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B871">
+        <v>13</v>
+      </c>
+      <c r="C871" t="s">
+        <v>1695</v>
+      </c>
+      <c r="D871" t="s">
+        <v>1696</v>
+      </c>
+    </row>
+    <row r="872" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A872" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B872">
+        <v>14</v>
+      </c>
+      <c r="C872" t="s">
+        <v>1697</v>
+      </c>
+      <c r="D872" t="s">
+        <v>1698</v>
+      </c>
+    </row>
+    <row r="873" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A873" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B873">
+        <v>15</v>
+      </c>
+      <c r="C873" t="s">
+        <v>1699</v>
+      </c>
+      <c r="D873" t="s">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="874" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A874" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B874">
+        <v>16</v>
+      </c>
+      <c r="C874" t="s">
+        <v>1474</v>
+      </c>
+      <c r="D874" t="s">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="875" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A875" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B875">
+        <v>17</v>
+      </c>
+      <c r="C875" t="s">
+        <v>1701</v>
+      </c>
+      <c r="D875" t="s">
+        <v>1702</v>
+      </c>
+    </row>
+    <row r="876" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A876" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B876">
+        <v>18</v>
+      </c>
+      <c r="C876" t="s">
+        <v>1703</v>
+      </c>
+      <c r="D876" t="s">
+        <v>1704</v>
+      </c>
+    </row>
+    <row r="877" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A877" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B877">
+        <v>19</v>
+      </c>
+      <c r="C877" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D877" t="s">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="878" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A878" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B878">
+        <v>20</v>
+      </c>
+      <c r="C878" t="s">
+        <v>1707</v>
+      </c>
+      <c r="D878" t="s">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="879" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A879" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B879">
+        <v>21</v>
+      </c>
+      <c r="C879" t="s">
+        <v>1709</v>
+      </c>
+      <c r="D879" t="s">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="880" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A880" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B880">
+        <v>22</v>
+      </c>
+      <c r="C880" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D880" t="s">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="881" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B881">
+        <v>23</v>
+      </c>
+      <c r="C881" t="s">
+        <v>1713</v>
+      </c>
+      <c r="D881" t="s">
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="882" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B882">
+        <v>24</v>
+      </c>
+      <c r="C882" t="s">
+        <v>1715</v>
+      </c>
+      <c r="D882" t="s">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="883" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B883">
+        <v>25</v>
+      </c>
+      <c r="C883" t="s">
+        <v>1717</v>
+      </c>
+      <c r="D883" t="s">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="884" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B884">
+        <v>26</v>
+      </c>
+      <c r="C884" t="s">
+        <v>1719</v>
+      </c>
+      <c r="D884" t="s">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="885" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B885">
+        <v>27</v>
+      </c>
+      <c r="C885" t="s">
+        <v>1721</v>
+      </c>
+      <c r="D885" t="s">
+        <v>1722</v>
+      </c>
+    </row>
+    <row r="886" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B886">
+        <v>28</v>
+      </c>
+      <c r="C886" t="s">
+        <v>1723</v>
+      </c>
+      <c r="D886" t="s">
+        <v>1724</v>
+      </c>
+    </row>
+    <row r="887" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B887">
+        <v>29</v>
+      </c>
+      <c r="C887" t="s">
+        <v>1725</v>
+      </c>
+      <c r="D887" t="s">
+        <v>1726</v>
+      </c>
+    </row>
+    <row r="888" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B888">
+        <v>30</v>
+      </c>
+      <c r="C888" t="s">
+        <v>1727</v>
+      </c>
+      <c r="D888" t="s">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="889" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B889">
+        <v>31</v>
+      </c>
+      <c r="C889" t="s">
+        <v>1729</v>
+      </c>
+      <c r="D889" t="s">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="890" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B890">
+        <v>32</v>
+      </c>
+      <c r="C890" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D890" t="s">
+        <v>1647</v>
+      </c>
+    </row>
+    <row r="891" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B891">
+        <v>33</v>
+      </c>
+      <c r="C891" t="s">
+        <v>1648</v>
+      </c>
+      <c r="D891" t="s">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="892" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B892">
+        <v>34</v>
+      </c>
+      <c r="C892" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D892" t="s">
+        <v>1653</v>
+      </c>
+    </row>
+    <row r="893" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B893">
+        <v>35</v>
+      </c>
+      <c r="C893" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D893" t="s">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="894" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B894">
+        <v>36</v>
+      </c>
+      <c r="C894" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D894" t="s">
+        <v>1655</v>
+      </c>
+    </row>
+    <row r="895" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B895">
+        <v>37</v>
+      </c>
+      <c r="C895" t="s">
+        <v>1731</v>
+      </c>
+      <c r="D895" t="s">
+        <v>1732</v>
+      </c>
+    </row>
+    <row r="896" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B896">
+        <v>38</v>
+      </c>
+      <c r="C896" t="s">
+        <v>1733</v>
+      </c>
+      <c r="D896" t="s">
+        <v>1734</v>
+      </c>
+    </row>
+    <row r="897" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A897" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B897">
+        <v>39</v>
+      </c>
+      <c r="C897" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D897" t="s">
+        <v>1736</v>
+      </c>
+    </row>
+    <row r="898" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A898" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B898">
+        <v>40</v>
+      </c>
+      <c r="C898" t="s">
+        <v>1478</v>
+      </c>
+      <c r="D898" t="s">
+        <v>1479</v>
+      </c>
+    </row>
+    <row r="899" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B899">
+        <v>41</v>
+      </c>
+      <c r="C899" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D899" t="s">
+        <v>1738</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D585" xr:uid="{9AE8CAB7-A756-48C6-BF24-AF23F25D3BD8}"/>
   <conditionalFormatting sqref="C1:C1048576">

</xml_diff>